<commit_message>
Extracted Sheet 2 Data
</commit_message>
<xml_diff>
--- a/data/sheet2.xlsx
+++ b/data/sheet2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shekarnatarajan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUMIO_AI\orchestro-carrier-search\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C570090A-B73D-274E-9F50-DB5F8C93DD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2AD946-9E3A-495D-83BA-A2F08E49557D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{42DB201B-0F71-2A4B-A2CD-9D602783218E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{42DB201B-0F71-2A4B-A2CD-9D602783218E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,38 +27,14 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </valueMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>LaserShip - lasership.com</t>
   </si>
@@ -510,10 +486,7 @@
     <t>Carey Limousine - carey.com</t>
   </si>
   <si>
-    <t>ReplyForward</t>
-  </si>
-  <si>
-    <t>Add reaction</t>
+    <t>Links</t>
   </si>
 </sst>
 </file>
@@ -598,64 +571,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
 </file>
 
 <file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
@@ -981,939 +896,938 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ACB51D-1558-AF4B-AF09-C935B7457145}">
-  <dimension ref="A1:B153"/>
+  <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144" s="1" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="1" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="1" t="s">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="1" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="1" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="2"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="4" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="2"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="4"/>
-      <c r="B153" s="2" t="s">
-        <v>151</v>
-      </c>
+      <c r="B153" s="3"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="4"/>
+      <c r="B154" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A152:A153"/>
+    <mergeCell ref="A153:A154"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://www.lasership.com/" xr:uid="{0092CE2D-CCA5-254C-8D28-679905CC3BBE}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://www.ontrac.com/" xr:uid="{A1552006-15A1-624F-AF72-AC33C66F88B7}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://www.lso.com/" xr:uid="{E2EF5840-E310-9446-9A7A-A2A52316BD56}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://courierexpress.net/" xr:uid="{558F5CDA-B8ED-E646-96A6-963276717F7B}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://www.udsgroup.com/" xr:uid="{1F440A0D-D7C6-284C-8BDA-9466C8372726}"/>
-    <hyperlink ref="A6" r:id="rId6" display="https://www.tforcelogistics.com/" xr:uid="{14C793FE-E726-924B-A8A5-C720B53E704A}"/>
-    <hyperlink ref="A7" r:id="rId7" display="http://www.uscargoonline.com/" xr:uid="{038C56DA-97B7-B041-A395-BDBB6DE63815}"/>
-    <hyperlink ref="A8" r:id="rId8" display="https://www.dynamex.com/" xr:uid="{77BFC4BD-1199-B743-A808-56BA76F2141E}"/>
-    <hyperlink ref="A9" r:id="rId9" display="https://www.velocityexpress.com/" xr:uid="{419B5443-89C7-604D-9AE8-B1513D13005C}"/>
-    <hyperlink ref="A10" r:id="rId10" display="http://www.courier-connection.com/" xr:uid="{349C2E28-C227-7441-B1D8-0C01757BBDB1}"/>
-    <hyperlink ref="A11" r:id="rId11" display="https://www.cdlusa.com/" xr:uid="{A5178459-ED77-0444-A0B1-BC3CA83F5D59}"/>
-    <hyperlink ref="A12" r:id="rId12" display="https://pace-usa.com/" xr:uid="{36157138-4478-3445-B790-E7DF22C6103D}"/>
-    <hyperlink ref="A13" r:id="rId13" display="https://www.tforcefreight.com/" xr:uid="{AF44F56B-2EB0-7349-99E2-E4BE757618D6}"/>
-    <hyperlink ref="A14" r:id="rId14" display="https://www.speedeedelivery.com/" xr:uid="{F7EC0E48-A5EE-4B4D-B234-3254D16A5D20}"/>
-    <hyperlink ref="A15" r:id="rId15" display="http://www.valleycourier.com/" xr:uid="{54723D59-656B-C74C-B7C6-6A7823A9A402}"/>
-    <hyperlink ref="A16" r:id="rId16" display="http://www.usmessenger.com/" xr:uid="{E4F61D77-956E-4A4C-B125-B058AFA99BE9}"/>
-    <hyperlink ref="A17" r:id="rId17" display="http://www.gsodirect.com/" xr:uid="{48DA19D3-E363-A147-B8BC-889C268AD45C}"/>
-    <hyperlink ref="A18" r:id="rId18" display="https://www.pittohio.com/" xr:uid="{4440EEF2-3A21-454E-B89F-7182CB915034}"/>
-    <hyperlink ref="A19" r:id="rId19" display="http://rrdonnelley.com/logistics" xr:uid="{670DD3BF-0C4A-5C4A-A5B3-39B79A773117}"/>
-    <hyperlink ref="A20" r:id="rId20" display="http://www.samedaydelivery.com/" xr:uid="{5C290A22-7882-1F4D-B185-6736C4D64179}"/>
-    <hyperlink ref="A21" r:id="rId21" display="http://www.reddyice.com/" xr:uid="{E2B4BA4B-F9D7-AE48-B63D-7D1388546CFA}"/>
-    <hyperlink ref="A22" r:id="rId22" display="https://gouspack.com/" xr:uid="{37480ACC-BFEB-6440-BEE3-4092A289814F}"/>
-    <hyperlink ref="A23" r:id="rId23" display="http://www.hotshot-deliveries.com/" xr:uid="{FFF32FD5-DEF8-F542-AFC3-B150B9E1443F}"/>
-    <hyperlink ref="A24" r:id="rId24" display="https://capexspress.com/" xr:uid="{DA30A1FB-4773-3E4E-A347-E496391F6CB6}"/>
-    <hyperlink ref="A25" r:id="rId25" display="http://www.chicagomessenger.com/" xr:uid="{57F6017F-FCBB-F243-BE83-69CF2CE21892}"/>
-    <hyperlink ref="A26" r:id="rId26" display="http://www.soniccourier.com/" xr:uid="{B087EA9D-9071-4448-9D45-B58F63A821A7}"/>
-    <hyperlink ref="A27" r:id="rId27" display="https://www.clutchcourier.com/" xr:uid="{C0D3FDD5-DDD8-CD41-868F-042329F83B78}"/>
-    <hyperlink ref="A28" r:id="rId28" display="https://1stchoicedelivery.com/" xr:uid="{12B08B03-ACC5-9448-AC59-F18B0A0EC69A}"/>
-    <hyperlink ref="A29" r:id="rId29" display="https://www.diligentusa.com/" xr:uid="{270B90E9-83ED-4145-BC2F-50DD15BE8F01}"/>
-    <hyperlink ref="A30" r:id="rId30" display="https://www.mobileair.com/" xr:uid="{49BB0922-93C8-EF4A-AAD4-B9CD98C6F996}"/>
-    <hyperlink ref="A31" r:id="rId31" display="http://www.hotlinedelivers.com/" xr:uid="{DA1B5769-1C0D-2547-9F3A-BCD1D4F3E076}"/>
-    <hyperlink ref="A32" r:id="rId32" display="https://www.priorityexpress.com/" xr:uid="{C462EA3B-54AC-1A4E-B210-1746ECBD5C3D}"/>
-    <hyperlink ref="A33" r:id="rId33" display="http://www.jetexpress.com/" xr:uid="{993159F7-3C69-9D4A-B098-65B11AA0F88F}"/>
-    <hyperlink ref="A34" r:id="rId34" display="http://www.courierexpressne.com/" xr:uid="{31EE53E6-6C19-CD40-985F-A5CCB1C922C7}"/>
-    <hyperlink ref="A35" r:id="rId35" display="http://www.selectexp.com/" xr:uid="{2B1C0A75-62F7-4D4B-AB3D-D17AFA1FA510}"/>
-    <hyperlink ref="A36" r:id="rId36" display="http://www.westernpeakslogistics.com/" xr:uid="{FDA569DD-36E8-F346-98B3-5665C0FBE5D5}"/>
-    <hyperlink ref="A37" r:id="rId37" display="http://www.medspeed.com/" xr:uid="{A2D8869D-3FDD-A14E-8C74-C1977DA1257D}"/>
-    <hyperlink ref="A38" r:id="rId38" display="http://www.spartanlogistics.com/" xr:uid="{E08D22E7-448D-7341-BDA5-A78EDA1F0282}"/>
-    <hyperlink ref="A39" r:id="rId39" display="http://www.lanterdeliverysystems.com/" xr:uid="{7E644DB5-0B8D-DD43-B6E9-25480D250741}"/>
-    <hyperlink ref="A40" r:id="rId40" display="https://ironcladcourier.com/" xr:uid="{AE3D24E8-ABA5-FE45-B91F-D5637A3E7575}"/>
-    <hyperlink ref="A41" r:id="rId41" display="http://www.tukaway.com/" xr:uid="{F6C34EA1-47E9-364A-9182-3D131E702518}"/>
-    <hyperlink ref="A42" r:id="rId42" display="https://courierds.com/" xr:uid="{17EFE97A-9EB4-4D48-8D4E-B37DEB2DB2C3}"/>
-    <hyperlink ref="A43" r:id="rId43" display="https://www.expresscourierintl.com/" xr:uid="{A2EDF10A-4C46-A249-A2F3-2C2EE8B82190}"/>
-    <hyperlink ref="A44" r:id="rId44" display="https://alphalogistics.net/" xr:uid="{D93DCCB1-8FB2-D147-ACD0-DA984D844B39}"/>
-    <hyperlink ref="A45" r:id="rId45" display="https://www.citysprint.co.uk/" xr:uid="{B9FFCE0A-91CB-C742-8192-825F0EEE8E54}"/>
-    <hyperlink ref="A46" r:id="rId46" display="https://goflypigeon.com/" xr:uid="{1EB671B0-5CD4-8C4A-AE80-B9A89B482B68}"/>
-    <hyperlink ref="A47" r:id="rId47" display="https://www.priority.com/" xr:uid="{8F1CDFE8-B582-1047-9E13-A0D5554AAE29}"/>
-    <hyperlink ref="A48" r:id="rId48" display="https://www.corporatecouriers.net/" xr:uid="{EAC82308-28DB-FF4B-8F12-B318C2E1CF62}"/>
-    <hyperlink ref="A49" r:id="rId49" display="http://www.skynetworldwide.com/" xr:uid="{5351F509-69CC-CF41-B6AD-4C9FA182EBAE}"/>
-    <hyperlink ref="A50" r:id="rId50" display="https://www.tukawaycourier.com/" xr:uid="{5B156A8C-96F9-A540-8A9D-D3A860E69B00}"/>
-    <hyperlink ref="A51" r:id="rId51" display="https://bondedlogistics.com/" xr:uid="{198DE690-8853-6D4A-8551-32471925DAE3}"/>
-    <hyperlink ref="A52" r:id="rId52" display="https://customcouriersystems.com/" xr:uid="{9D3F6B5D-C10D-DE4F-A0FC-FBB569B9F24F}"/>
-    <hyperlink ref="A53" r:id="rId53" display="http://www.easternconnection.com/" xr:uid="{CDA14260-F1B4-9144-B210-82F0BDBFB36D}"/>
-    <hyperlink ref="A54" r:id="rId54" display="http://www.am-tran.com/" xr:uid="{05AB0F7B-3EFC-B242-B6FF-1A2D3BE38468}"/>
-    <hyperlink ref="A55" r:id="rId55" display="http://www.sunlinecourier.com/" xr:uid="{72B660A2-48DC-4247-9AB0-4AEE0668AEDC}"/>
-    <hyperlink ref="A56" r:id="rId56" display="http://www.professionalcourier.com/" xr:uid="{1ECB5CE3-64A0-674E-8FB9-F0979D63AFC0}"/>
-    <hyperlink ref="A57" r:id="rId57" display="https://spokesdc.com/" xr:uid="{A1694C5E-07B5-484E-BF03-A46B2E0534E2}"/>
-    <hyperlink ref="A58" r:id="rId58" display="http://www.kingcourier.com/" xr:uid="{72E41667-5D09-1A4A-A10A-13E0E3BF24DD}"/>
-    <hyperlink ref="A59" r:id="rId59" display="http://www.horizonlogistics.com/" xr:uid="{50DE3F42-2594-E04B-A7DA-953E93367FD4}"/>
-    <hyperlink ref="A60" r:id="rId60" display="https://www.eagleexpress.com/" xr:uid="{346A60D7-FEE9-4940-9D40-56D6E5089D42}"/>
-    <hyperlink ref="A61" r:id="rId61" display="http://www.kingdomcourier.com/" xr:uid="{A6C2A390-9BB7-554E-A77E-8FA32577980A}"/>
-    <hyperlink ref="A62" r:id="rId62" display="https://hdsexpress.com/" xr:uid="{2B1CE6E2-C998-4F4E-9911-7417660E6400}"/>
-    <hyperlink ref="A63" r:id="rId63" display="https://pelicandelivery.com/" xr:uid="{B91324B5-9FC6-894A-ABED-65574718E064}"/>
-    <hyperlink ref="A64" r:id="rId64" display="http://www.courierasap.com/" xr:uid="{69F6C280-8500-8745-95B3-80214AD455F8}"/>
-    <hyperlink ref="A65" r:id="rId65" display="http://www.skycourier.com/" xr:uid="{9A17C03A-04C7-4A44-A6A9-21F7680F517D}"/>
-    <hyperlink ref="A66" r:id="rId66" display="https://www.abccourier.com/" xr:uid="{46F65F7D-112D-F744-BE88-839D4B052BF3}"/>
-    <hyperlink ref="A67" r:id="rId67" display="http://www.quickdelivers.com/" xr:uid="{BB8F01ED-F0E0-D246-B45E-D864AC00843E}"/>
-    <hyperlink ref="A68" r:id="rId68" display="http://www.redlinecourier.com/" xr:uid="{3D61115B-399C-4B48-8050-1ED9E1216A41}"/>
-    <hyperlink ref="A69" r:id="rId69" display="https://www.trinitylogistics.com/" xr:uid="{94965BAD-B0BE-4E44-AE3F-6962C20F6657}"/>
-    <hyperlink ref="A70" r:id="rId70" display="http://www.ctclogistics.com/" xr:uid="{8B63DBB3-1620-0241-8459-8D58B18C7A50}"/>
-    <hyperlink ref="A71" r:id="rId71" display="http://www.marten.com/" xr:uid="{D01AD3BE-64C7-7748-9CD6-4016A1DB796E}"/>
-    <hyperlink ref="A72" r:id="rId72" display="https://www.westsideexpress.net/" xr:uid="{127B7AD6-B247-624F-B5FE-28D34212F527}"/>
-    <hyperlink ref="A73" r:id="rId73" display="https://milehiexpress.com/" xr:uid="{AA5EDB98-B410-144D-A1ED-48EC754D3BE2}"/>
-    <hyperlink ref="A74" r:id="rId74" display="https://www.abccourierservice.com/" xr:uid="{BBE5558F-F660-144C-8560-F37FF79AFCAB}"/>
-    <hyperlink ref="A75" r:id="rId75" display="http://www.cometdelivery.com/" xr:uid="{C4FE9A8B-1A35-A145-83D9-73F876EB8B01}"/>
-    <hyperlink ref="A76" r:id="rId76" display="http://www.americancourierservice.com/" xr:uid="{3480478A-801C-384A-885F-CF06A712EB6D}"/>
-    <hyperlink ref="A77" r:id="rId77" display="https://www.procourier.com/" xr:uid="{6FBFB7FF-0923-714D-BD19-62402574F2DD}"/>
-    <hyperlink ref="A78" r:id="rId78" display="https://www.rrts.com/" xr:uid="{78BC5DA5-A611-5F45-B0F0-5F10DE473A4F}"/>
-    <hyperlink ref="A79" r:id="rId79" display="https://www.xpo.com/" xr:uid="{6609E93E-39A0-9346-B240-2AAF82AC757A}"/>
-    <hyperlink ref="A80" r:id="rId80" display="http://www.landairexpress.com/" xr:uid="{2563FE43-02DF-7448-847D-43C0608A28ED}"/>
-    <hyperlink ref="A81" r:id="rId81" display="https://www.amexpediting.com/" xr:uid="{3082ED72-550C-FE42-8605-61E28D53D9C7}"/>
-    <hyperlink ref="A82" r:id="rId82" display="http://www.californiacourierservices.com/" xr:uid="{E693F396-B94B-2C46-813E-CFC4EA64E8C5}"/>
-    <hyperlink ref="A83" r:id="rId83" display="http://www.jetdelivery.com/" xr:uid="{03A2A585-C2D9-F44B-80BD-40C5B76298A1}"/>
-    <hyperlink ref="A84" r:id="rId84" display="http://www.aeexp.com/" xr:uid="{7892E5F8-D338-224F-8601-6DF95598C903}"/>
-    <hyperlink ref="A85" r:id="rId85" display="http://www.mccollisters.com/" xr:uid="{74598202-682B-BA48-B7D2-05475F32A498}"/>
-    <hyperlink ref="A86" r:id="rId86" display="https://www.sterlingtransportation.com/" xr:uid="{36F7985C-8ABD-3A4D-8BE1-BE57F3ECFC3A}"/>
-    <hyperlink ref="A87" r:id="rId87" display="http://www.pegasuslogistics.com/" xr:uid="{B0E90E67-6A1B-7E4B-9891-3D3D6076B7C9}"/>
-    <hyperlink ref="A88" r:id="rId88" display="https://www.protrans.com/" xr:uid="{2B79B6A9-9CDD-864A-B0FC-2D134FCBCF8B}"/>
-    <hyperlink ref="A89" r:id="rId89" display="http://www.shepardtrucking.com/" xr:uid="{04DF2D92-07F4-1D43-AC33-F9E958E05A57}"/>
-    <hyperlink ref="A90" r:id="rId90" display="http://www.capitaldeliverysystems.com/" xr:uid="{4346CED9-C4EF-D245-83E4-CD4AF4A49EDA}"/>
-    <hyperlink ref="A91" r:id="rId91" display="https://www.swifttrans.com/" xr:uid="{85EFA135-460A-D045-A0A6-2ED3F28A9BD0}"/>
-    <hyperlink ref="A92" r:id="rId92" display="http://www.daylighttransport.com/" xr:uid="{9D04F818-4DAC-CE40-860A-A7CAD19A8B4F}"/>
-    <hyperlink ref="A93" r:id="rId93" display="http://www.jaguarlogistics.com/" xr:uid="{5B53DA21-CCA5-6C47-9FF4-DB3D4A842A55}"/>
-    <hyperlink ref="A94" r:id="rId94" display="http://www.3pd.com/" xr:uid="{CD1DF48B-13EF-F943-A5DD-C1509EC67C18}"/>
-    <hyperlink ref="A95" r:id="rId95" display="http://www.interstatecourier.com/" xr:uid="{E8BE706B-DC18-4A40-BE7A-C6600F976E5E}"/>
-    <hyperlink ref="A96" r:id="rId96" display="http://www.uscargocourier.com/" xr:uid="{B447438C-AD8A-6C45-B7F1-B812EBE32A6A}"/>
-    <hyperlink ref="A97" r:id="rId97" display="http://www.nationallogisticsgroup.com/" xr:uid="{99633C94-B636-5941-9EAD-C7988D2EB60A}"/>
-    <hyperlink ref="A98" r:id="rId98" display="http://www.rmx.com/" xr:uid="{87D13EF8-8C2F-AB49-84B8-CCE88BA9BAC9}"/>
-    <hyperlink ref="A99" r:id="rId99" display="https://www.globaltranz.com/" xr:uid="{99DBCACC-3831-CC4C-A0A3-E715CAED71A4}"/>
-    <hyperlink ref="A100" r:id="rId100" display="http://www.estes-express.com/" xr:uid="{90EB180E-2DB8-A04F-A7C6-96C49C0CF18B}"/>
-    <hyperlink ref="A101" r:id="rId101" display="http://www.centralfreight.com/" xr:uid="{88136DC6-8D22-844F-ADC0-B3744ACE74BD}"/>
-    <hyperlink ref="A102" r:id="rId102" display="http://www.mtnvly.com/" xr:uid="{ED5BE652-261A-6740-880D-05C69CA79873}"/>
-    <hyperlink ref="A103" r:id="rId103" display="http://www.crosscountrycourier.com/" xr:uid="{C757318B-60C8-334C-9A87-FB7377CD4F06}"/>
-    <hyperlink ref="A104" r:id="rId104" display="http://www.corporatecouriers.com/" xr:uid="{8621FB21-D785-6244-BA82-6B07E4A071A8}"/>
-    <hyperlink ref="A105" r:id="rId105" display="http://www.smart-delivery.com/" xr:uid="{722919A5-1555-1947-B412-E4B139EA599C}"/>
-    <hyperlink ref="A106" r:id="rId106" display="http://www.cityexp.com/" xr:uid="{B161F0F5-8895-DC4C-9CC2-AAA682FABD3E}"/>
-    <hyperlink ref="A107" r:id="rId107" display="https://dedicatedlogistics.com/" xr:uid="{9A0605E8-252B-1349-8982-3CEFD005D130}"/>
-    <hyperlink ref="A108" r:id="rId108" display="http://www.firstclasscourier.com/" xr:uid="{362AF675-9AA0-2B48-A9AC-DD95A150B0A3}"/>
-    <hyperlink ref="A109" r:id="rId109" display="http://www.sprintcourier.com/" xr:uid="{493CC60E-DA46-A043-B446-2AE6141CD224}"/>
-    <hyperlink ref="A110" r:id="rId110" display="http://www.samedaydelivers.com/" xr:uid="{0434A8F6-D2E9-3D44-8D65-12B9730C2BD7}"/>
-    <hyperlink ref="A111" r:id="rId111" display="https://www.truenorthlogistics.com/" xr:uid="{46DE5B1C-8128-E242-8EB4-07D8BBEE9695}"/>
-    <hyperlink ref="A112" r:id="rId112" display="https://goshare.co/" xr:uid="{31DE32CC-3670-1941-97B3-69C074C05E05}"/>
-    <hyperlink ref="A113" r:id="rId113" display="http://www.mulesoftlogistics.com/" xr:uid="{96D3F76A-733B-DC4C-BD2F-86BDCA63F6D6}"/>
-    <hyperlink ref="A114" r:id="rId114" display="http://www.quickcourier.com/" xr:uid="{04F0F538-B5EE-2D4A-AD90-EA09C7B45C38}"/>
-    <hyperlink ref="A115" r:id="rId115" display="http://www.bonded-transportation.com/" xr:uid="{0CDDF333-6076-404C-B756-BB0B85B2FA8A}"/>
-    <hyperlink ref="A116" r:id="rId116" display="http://www.uscourier.com/" xr:uid="{29735F40-4722-A946-BAC8-923A74C6F302}"/>
-    <hyperlink ref="A117" r:id="rId117" display="http://www.expressitdelivery.com/" xr:uid="{D6AF596D-3BB5-814A-9501-A2BCAEC7B465}"/>
-    <hyperlink ref="A118" r:id="rId118" display="http://www.michiganlogistics.com/" xr:uid="{2C559D59-04BA-3648-A305-DF8DB2AC2811}"/>
-    <hyperlink ref="A119" r:id="rId119" display="http://www.easexpress.com/" xr:uid="{E6C0A4DF-4B29-6443-AB8C-0D7E8AC97BEF}"/>
-    <hyperlink ref="A120" r:id="rId120" display="http://www.sherdeltransfer.com/" xr:uid="{BB6C5ACA-C061-8240-8D44-F448DFA325BD}"/>
-    <hyperlink ref="A121" r:id="rId121" display="http://www.corporatetransit.com/" xr:uid="{D3526926-F27A-524E-9227-624BD1B37061}"/>
-    <hyperlink ref="A122" r:id="rId122" display="https://eastcoastlogistics.com/" xr:uid="{C0AE48AF-9E3D-2249-910F-D019AFB537B0}"/>
-    <hyperlink ref="A123" r:id="rId123" display="https://point2pointglobal.com/" xr:uid="{689E3A35-F35F-7C43-B50E-5CC93BBA5900}"/>
-    <hyperlink ref="A124" r:id="rId124" display="https://ecouriergroup.com/" xr:uid="{DBC1B9D8-272C-E348-9725-7ED00BCA1115}"/>
-    <hyperlink ref="A125" r:id="rId125" display="http://www.westcoastlogistics.net/" xr:uid="{DC10D6A4-C444-4E49-98DC-3489E2BCF9D4}"/>
-    <hyperlink ref="A126" r:id="rId126" display="https://www.shipmercury.com/" xr:uid="{D034C736-C615-3248-8C3B-2EBE3434CA60}"/>
-    <hyperlink ref="A127" r:id="rId127" display="https://www.ezcourier.com/" xr:uid="{16C9040A-BC17-CC45-97B5-9C5CD8DDDF8D}"/>
-    <hyperlink ref="A128" r:id="rId128" display="http://www.regionalexpressinc.com/" xr:uid="{B95E5445-9E31-3242-A954-7DDAB76BAED1}"/>
-    <hyperlink ref="A129" r:id="rId129" display="http://www.citywidecouriers.com/" xr:uid="{A30FBA8A-7528-1E4B-89F0-5FF7D173D1ED}"/>
-    <hyperlink ref="A130" r:id="rId130" display="https://www.monarchdelivery.com/" xr:uid="{6A1A2A79-1A66-C54D-9629-6926B684CC31}"/>
-    <hyperlink ref="A131" r:id="rId131" display="http://www.capitolexpressinc.com/" xr:uid="{89E9BCFC-82D6-8A43-9A30-5CB3A369A7E8}"/>
-    <hyperlink ref="A132" r:id="rId132" display="http://www.jrsexpressdelivery.com/" xr:uid="{7FDEC950-B4AA-CA4F-A1FC-8596478C50FA}"/>
-    <hyperlink ref="A133" r:id="rId133" display="https://www.acecourier.com/" xr:uid="{5A631D9C-B941-1C49-B565-F29CEA731A1D}"/>
-    <hyperlink ref="A134" r:id="rId134" display="http://www.parcelsinc.com/" xr:uid="{67312458-7442-484A-91C2-A3E626C92A1F}"/>
-    <hyperlink ref="A135" r:id="rId135" display="http://www.hollandregional.com/" xr:uid="{222F5D8B-BF76-FF48-AF9D-163F0A7269C1}"/>
-    <hyperlink ref="A136" r:id="rId136" display="http://www.prioritydispatch.com/" xr:uid="{D1AC3139-4358-6548-9998-818FE967ECFC}"/>
-    <hyperlink ref="A137" r:id="rId137" display="http://www.hackbarthdelivery.com/" xr:uid="{09764DC2-E2CF-254F-A682-0ACA6148D95E}"/>
-    <hyperlink ref="A138" r:id="rId138" display="https://www.shipgreyhound.com/" xr:uid="{458FAEF0-5C87-F042-AC78-7DB88C3EE0D4}"/>
-    <hyperlink ref="A139" r:id="rId139" display="http://www.bonneydelivery.com/" xr:uid="{1ACCF52D-5BC2-5549-BF6D-8366607790BD}"/>
-    <hyperlink ref="A140" r:id="rId140" display="http://www.shamrockexpress.com/" xr:uid="{75C59A68-676A-F649-B278-73E5ED1BF652}"/>
-    <hyperlink ref="A141" r:id="rId141" display="https://www.nationwideexpress.com/" xr:uid="{4E40ED77-558B-4148-A9E7-B1D55B27FA4B}"/>
-    <hyperlink ref="A142" r:id="rId142" display="http://www.metro-courier.com/" xr:uid="{E1C71248-40B0-9048-9175-0E86150D47F3}"/>
-    <hyperlink ref="A143" r:id="rId143" display="https://www.specializedexpress.com/" xr:uid="{2BC6C542-5FE7-1C44-A4B9-83648F9539EC}"/>
-    <hyperlink ref="A144" r:id="rId144" display="http://www.jetlinelogistics.com/" xr:uid="{3CF7FA22-5025-B24C-962A-F61DA85FAD55}"/>
-    <hyperlink ref="A145" r:id="rId145" display="http://www.swfreight.com/" xr:uid="{251B3CD1-3FCB-DD41-8F89-EC35455A7D0D}"/>
-    <hyperlink ref="A146" r:id="rId146" display="http://www.bluestreakcouriers.com/" xr:uid="{12F50950-E72F-9C4A-8515-46F56CC6F8E9}"/>
-    <hyperlink ref="A147" r:id="rId147" display="https://www.smtl.com/" xr:uid="{B62C4422-8395-2743-8C09-709ADD604246}"/>
-    <hyperlink ref="A148" r:id="rId148" display="http://www.americanlc.com/" xr:uid="{D1CAA362-9669-8042-9634-8D9329EA51A1}"/>
-    <hyperlink ref="A149" r:id="rId149" display="https://www.starfreight.com/" xr:uid="{2F0923AD-C1D4-5044-BFE6-0009D935E4A5}"/>
-    <hyperlink ref="A150" r:id="rId150" display="http://www.carey.com/" xr:uid="{97EC126C-117C-D141-B865-5445A0C376FC}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.lasership.com/" xr:uid="{0092CE2D-CCA5-254C-8D28-679905CC3BBE}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.ontrac.com/" xr:uid="{A1552006-15A1-624F-AF72-AC33C66F88B7}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://www.lso.com/" xr:uid="{E2EF5840-E310-9446-9A7A-A2A52316BD56}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://courierexpress.net/" xr:uid="{558F5CDA-B8ED-E646-96A6-963276717F7B}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.udsgroup.com/" xr:uid="{1F440A0D-D7C6-284C-8BDA-9466C8372726}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.tforcelogistics.com/" xr:uid="{14C793FE-E726-924B-A8A5-C720B53E704A}"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://www.uscargoonline.com/" xr:uid="{038C56DA-97B7-B041-A395-BDBB6DE63815}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.dynamex.com/" xr:uid="{77BFC4BD-1199-B743-A808-56BA76F2141E}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.velocityexpress.com/" xr:uid="{419B5443-89C7-604D-9AE8-B1513D13005C}"/>
+    <hyperlink ref="A11" r:id="rId10" display="http://www.courier-connection.com/" xr:uid="{349C2E28-C227-7441-B1D8-0C01757BBDB1}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://www.cdlusa.com/" xr:uid="{A5178459-ED77-0444-A0B1-BC3CA83F5D59}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://pace-usa.com/" xr:uid="{36157138-4478-3445-B790-E7DF22C6103D}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://www.tforcefreight.com/" xr:uid="{AF44F56B-2EB0-7349-99E2-E4BE757618D6}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://www.speedeedelivery.com/" xr:uid="{F7EC0E48-A5EE-4B4D-B234-3254D16A5D20}"/>
+    <hyperlink ref="A16" r:id="rId15" display="http://www.valleycourier.com/" xr:uid="{54723D59-656B-C74C-B7C6-6A7823A9A402}"/>
+    <hyperlink ref="A17" r:id="rId16" display="http://www.usmessenger.com/" xr:uid="{E4F61D77-956E-4A4C-B125-B058AFA99BE9}"/>
+    <hyperlink ref="A18" r:id="rId17" display="http://www.gsodirect.com/" xr:uid="{48DA19D3-E363-A147-B8BC-889C268AD45C}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://www.pittohio.com/" xr:uid="{4440EEF2-3A21-454E-B89F-7182CB915034}"/>
+    <hyperlink ref="A20" r:id="rId19" display="http://rrdonnelley.com/logistics" xr:uid="{670DD3BF-0C4A-5C4A-A5B3-39B79A773117}"/>
+    <hyperlink ref="A21" r:id="rId20" display="http://www.samedaydelivery.com/" xr:uid="{5C290A22-7882-1F4D-B185-6736C4D64179}"/>
+    <hyperlink ref="A22" r:id="rId21" display="http://www.reddyice.com/" xr:uid="{E2B4BA4B-F9D7-AE48-B63D-7D1388546CFA}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://gouspack.com/" xr:uid="{37480ACC-BFEB-6440-BEE3-4092A289814F}"/>
+    <hyperlink ref="A24" r:id="rId23" display="http://www.hotshot-deliveries.com/" xr:uid="{FFF32FD5-DEF8-F542-AFC3-B150B9E1443F}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://capexspress.com/" xr:uid="{DA30A1FB-4773-3E4E-A347-E496391F6CB6}"/>
+    <hyperlink ref="A26" r:id="rId25" display="http://www.chicagomessenger.com/" xr:uid="{57F6017F-FCBB-F243-BE83-69CF2CE21892}"/>
+    <hyperlink ref="A27" r:id="rId26" display="http://www.soniccourier.com/" xr:uid="{B087EA9D-9071-4448-9D45-B58F63A821A7}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://www.clutchcourier.com/" xr:uid="{C0D3FDD5-DDD8-CD41-868F-042329F83B78}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://1stchoicedelivery.com/" xr:uid="{12B08B03-ACC5-9448-AC59-F18B0A0EC69A}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://www.diligentusa.com/" xr:uid="{270B90E9-83ED-4145-BC2F-50DD15BE8F01}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://www.mobileair.com/" xr:uid="{49BB0922-93C8-EF4A-AAD4-B9CD98C6F996}"/>
+    <hyperlink ref="A32" r:id="rId31" display="http://www.hotlinedelivers.com/" xr:uid="{DA1B5769-1C0D-2547-9F3A-BCD1D4F3E076}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://www.priorityexpress.com/" xr:uid="{C462EA3B-54AC-1A4E-B210-1746ECBD5C3D}"/>
+    <hyperlink ref="A34" r:id="rId33" display="http://www.jetexpress.com/" xr:uid="{993159F7-3C69-9D4A-B098-65B11AA0F88F}"/>
+    <hyperlink ref="A35" r:id="rId34" display="http://www.courierexpressne.com/" xr:uid="{31EE53E6-6C19-CD40-985F-A5CCB1C922C7}"/>
+    <hyperlink ref="A36" r:id="rId35" display="http://www.selectexp.com/" xr:uid="{2B1C0A75-62F7-4D4B-AB3D-D17AFA1FA510}"/>
+    <hyperlink ref="A37" r:id="rId36" display="http://www.westernpeakslogistics.com/" xr:uid="{FDA569DD-36E8-F346-98B3-5665C0FBE5D5}"/>
+    <hyperlink ref="A38" r:id="rId37" display="http://www.medspeed.com/" xr:uid="{A2D8869D-3FDD-A14E-8C74-C1977DA1257D}"/>
+    <hyperlink ref="A39" r:id="rId38" display="http://www.spartanlogistics.com/" xr:uid="{E08D22E7-448D-7341-BDA5-A78EDA1F0282}"/>
+    <hyperlink ref="A40" r:id="rId39" display="http://www.lanterdeliverysystems.com/" xr:uid="{7E644DB5-0B8D-DD43-B6E9-25480D250741}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://ironcladcourier.com/" xr:uid="{AE3D24E8-ABA5-FE45-B91F-D5637A3E7575}"/>
+    <hyperlink ref="A42" r:id="rId41" display="http://www.tukaway.com/" xr:uid="{F6C34EA1-47E9-364A-9182-3D131E702518}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://courierds.com/" xr:uid="{17EFE97A-9EB4-4D48-8D4E-B37DEB2DB2C3}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://www.expresscourierintl.com/" xr:uid="{A2EDF10A-4C46-A249-A2F3-2C2EE8B82190}"/>
+    <hyperlink ref="A45" r:id="rId44" display="https://alphalogistics.net/" xr:uid="{D93DCCB1-8FB2-D147-ACD0-DA984D844B39}"/>
+    <hyperlink ref="A46" r:id="rId45" display="https://www.citysprint.co.uk/" xr:uid="{B9FFCE0A-91CB-C742-8192-825F0EEE8E54}"/>
+    <hyperlink ref="A47" r:id="rId46" display="https://goflypigeon.com/" xr:uid="{1EB671B0-5CD4-8C4A-AE80-B9A89B482B68}"/>
+    <hyperlink ref="A48" r:id="rId47" display="https://www.priority.com/" xr:uid="{8F1CDFE8-B582-1047-9E13-A0D5554AAE29}"/>
+    <hyperlink ref="A49" r:id="rId48" display="https://www.corporatecouriers.net/" xr:uid="{EAC82308-28DB-FF4B-8F12-B318C2E1CF62}"/>
+    <hyperlink ref="A50" r:id="rId49" display="http://www.skynetworldwide.com/" xr:uid="{5351F509-69CC-CF41-B6AD-4C9FA182EBAE}"/>
+    <hyperlink ref="A51" r:id="rId50" display="https://www.tukawaycourier.com/" xr:uid="{5B156A8C-96F9-A540-8A9D-D3A860E69B00}"/>
+    <hyperlink ref="A52" r:id="rId51" display="https://bondedlogistics.com/" xr:uid="{198DE690-8853-6D4A-8551-32471925DAE3}"/>
+    <hyperlink ref="A53" r:id="rId52" display="https://customcouriersystems.com/" xr:uid="{9D3F6B5D-C10D-DE4F-A0FC-FBB569B9F24F}"/>
+    <hyperlink ref="A54" r:id="rId53" display="http://www.easternconnection.com/" xr:uid="{CDA14260-F1B4-9144-B210-82F0BDBFB36D}"/>
+    <hyperlink ref="A55" r:id="rId54" display="http://www.am-tran.com/" xr:uid="{05AB0F7B-3EFC-B242-B6FF-1A2D3BE38468}"/>
+    <hyperlink ref="A56" r:id="rId55" display="http://www.sunlinecourier.com/" xr:uid="{72B660A2-48DC-4247-9AB0-4AEE0668AEDC}"/>
+    <hyperlink ref="A57" r:id="rId56" display="http://www.professionalcourier.com/" xr:uid="{1ECB5CE3-64A0-674E-8FB9-F0979D63AFC0}"/>
+    <hyperlink ref="A58" r:id="rId57" display="https://spokesdc.com/" xr:uid="{A1694C5E-07B5-484E-BF03-A46B2E0534E2}"/>
+    <hyperlink ref="A59" r:id="rId58" display="http://www.kingcourier.com/" xr:uid="{72E41667-5D09-1A4A-A10A-13E0E3BF24DD}"/>
+    <hyperlink ref="A60" r:id="rId59" display="http://www.horizonlogistics.com/" xr:uid="{50DE3F42-2594-E04B-A7DA-953E93367FD4}"/>
+    <hyperlink ref="A61" r:id="rId60" display="https://www.eagleexpress.com/" xr:uid="{346A60D7-FEE9-4940-9D40-56D6E5089D42}"/>
+    <hyperlink ref="A62" r:id="rId61" display="http://www.kingdomcourier.com/" xr:uid="{A6C2A390-9BB7-554E-A77E-8FA32577980A}"/>
+    <hyperlink ref="A63" r:id="rId62" display="https://hdsexpress.com/" xr:uid="{2B1CE6E2-C998-4F4E-9911-7417660E6400}"/>
+    <hyperlink ref="A64" r:id="rId63" display="https://pelicandelivery.com/" xr:uid="{B91324B5-9FC6-894A-ABED-65574718E064}"/>
+    <hyperlink ref="A65" r:id="rId64" display="http://www.courierasap.com/" xr:uid="{69F6C280-8500-8745-95B3-80214AD455F8}"/>
+    <hyperlink ref="A66" r:id="rId65" display="http://www.skycourier.com/" xr:uid="{9A17C03A-04C7-4A44-A6A9-21F7680F517D}"/>
+    <hyperlink ref="A67" r:id="rId66" display="https://www.abccourier.com/" xr:uid="{46F65F7D-112D-F744-BE88-839D4B052BF3}"/>
+    <hyperlink ref="A68" r:id="rId67" display="http://www.quickdelivers.com/" xr:uid="{BB8F01ED-F0E0-D246-B45E-D864AC00843E}"/>
+    <hyperlink ref="A69" r:id="rId68" display="http://www.redlinecourier.com/" xr:uid="{3D61115B-399C-4B48-8050-1ED9E1216A41}"/>
+    <hyperlink ref="A70" r:id="rId69" display="https://www.trinitylogistics.com/" xr:uid="{94965BAD-B0BE-4E44-AE3F-6962C20F6657}"/>
+    <hyperlink ref="A71" r:id="rId70" display="http://www.ctclogistics.com/" xr:uid="{8B63DBB3-1620-0241-8459-8D58B18C7A50}"/>
+    <hyperlink ref="A72" r:id="rId71" display="http://www.marten.com/" xr:uid="{D01AD3BE-64C7-7748-9CD6-4016A1DB796E}"/>
+    <hyperlink ref="A73" r:id="rId72" display="https://www.westsideexpress.net/" xr:uid="{127B7AD6-B247-624F-B5FE-28D34212F527}"/>
+    <hyperlink ref="A74" r:id="rId73" display="https://milehiexpress.com/" xr:uid="{AA5EDB98-B410-144D-A1ED-48EC754D3BE2}"/>
+    <hyperlink ref="A75" r:id="rId74" display="https://www.abccourierservice.com/" xr:uid="{BBE5558F-F660-144C-8560-F37FF79AFCAB}"/>
+    <hyperlink ref="A76" r:id="rId75" display="http://www.cometdelivery.com/" xr:uid="{C4FE9A8B-1A35-A145-83D9-73F876EB8B01}"/>
+    <hyperlink ref="A77" r:id="rId76" display="http://www.americancourierservice.com/" xr:uid="{3480478A-801C-384A-885F-CF06A712EB6D}"/>
+    <hyperlink ref="A78" r:id="rId77" display="https://www.procourier.com/" xr:uid="{6FBFB7FF-0923-714D-BD19-62402574F2DD}"/>
+    <hyperlink ref="A79" r:id="rId78" display="https://www.rrts.com/" xr:uid="{78BC5DA5-A611-5F45-B0F0-5F10DE473A4F}"/>
+    <hyperlink ref="A80" r:id="rId79" display="https://www.xpo.com/" xr:uid="{6609E93E-39A0-9346-B240-2AAF82AC757A}"/>
+    <hyperlink ref="A81" r:id="rId80" display="http://www.landairexpress.com/" xr:uid="{2563FE43-02DF-7448-847D-43C0608A28ED}"/>
+    <hyperlink ref="A82" r:id="rId81" display="https://www.amexpediting.com/" xr:uid="{3082ED72-550C-FE42-8605-61E28D53D9C7}"/>
+    <hyperlink ref="A83" r:id="rId82" display="http://www.californiacourierservices.com/" xr:uid="{E693F396-B94B-2C46-813E-CFC4EA64E8C5}"/>
+    <hyperlink ref="A84" r:id="rId83" display="http://www.jetdelivery.com/" xr:uid="{03A2A585-C2D9-F44B-80BD-40C5B76298A1}"/>
+    <hyperlink ref="A85" r:id="rId84" display="http://www.aeexp.com/" xr:uid="{7892E5F8-D338-224F-8601-6DF95598C903}"/>
+    <hyperlink ref="A86" r:id="rId85" display="http://www.mccollisters.com/" xr:uid="{74598202-682B-BA48-B7D2-05475F32A498}"/>
+    <hyperlink ref="A87" r:id="rId86" display="https://www.sterlingtransportation.com/" xr:uid="{36F7985C-8ABD-3A4D-8BE1-BE57F3ECFC3A}"/>
+    <hyperlink ref="A88" r:id="rId87" display="http://www.pegasuslogistics.com/" xr:uid="{B0E90E67-6A1B-7E4B-9891-3D3D6076B7C9}"/>
+    <hyperlink ref="A89" r:id="rId88" display="https://www.protrans.com/" xr:uid="{2B79B6A9-9CDD-864A-B0FC-2D134FCBCF8B}"/>
+    <hyperlink ref="A90" r:id="rId89" display="http://www.shepardtrucking.com/" xr:uid="{04DF2D92-07F4-1D43-AC33-F9E958E05A57}"/>
+    <hyperlink ref="A91" r:id="rId90" display="http://www.capitaldeliverysystems.com/" xr:uid="{4346CED9-C4EF-D245-83E4-CD4AF4A49EDA}"/>
+    <hyperlink ref="A92" r:id="rId91" display="https://www.swifttrans.com/" xr:uid="{85EFA135-460A-D045-A0A6-2ED3F28A9BD0}"/>
+    <hyperlink ref="A93" r:id="rId92" display="http://www.daylighttransport.com/" xr:uid="{9D04F818-4DAC-CE40-860A-A7CAD19A8B4F}"/>
+    <hyperlink ref="A94" r:id="rId93" display="http://www.jaguarlogistics.com/" xr:uid="{5B53DA21-CCA5-6C47-9FF4-DB3D4A842A55}"/>
+    <hyperlink ref="A95" r:id="rId94" display="http://www.3pd.com/" xr:uid="{CD1DF48B-13EF-F943-A5DD-C1509EC67C18}"/>
+    <hyperlink ref="A96" r:id="rId95" display="http://www.interstatecourier.com/" xr:uid="{E8BE706B-DC18-4A40-BE7A-C6600F976E5E}"/>
+    <hyperlink ref="A97" r:id="rId96" display="http://www.uscargocourier.com/" xr:uid="{B447438C-AD8A-6C45-B7F1-B812EBE32A6A}"/>
+    <hyperlink ref="A98" r:id="rId97" display="http://www.nationallogisticsgroup.com/" xr:uid="{99633C94-B636-5941-9EAD-C7988D2EB60A}"/>
+    <hyperlink ref="A99" r:id="rId98" display="http://www.rmx.com/" xr:uid="{87D13EF8-8C2F-AB49-84B8-CCE88BA9BAC9}"/>
+    <hyperlink ref="A100" r:id="rId99" display="https://www.globaltranz.com/" xr:uid="{99DBCACC-3831-CC4C-A0A3-E715CAED71A4}"/>
+    <hyperlink ref="A101" r:id="rId100" display="http://www.estes-express.com/" xr:uid="{90EB180E-2DB8-A04F-A7C6-96C49C0CF18B}"/>
+    <hyperlink ref="A102" r:id="rId101" display="http://www.centralfreight.com/" xr:uid="{88136DC6-8D22-844F-ADC0-B3744ACE74BD}"/>
+    <hyperlink ref="A103" r:id="rId102" display="http://www.mtnvly.com/" xr:uid="{ED5BE652-261A-6740-880D-05C69CA79873}"/>
+    <hyperlink ref="A104" r:id="rId103" display="http://www.crosscountrycourier.com/" xr:uid="{C757318B-60C8-334C-9A87-FB7377CD4F06}"/>
+    <hyperlink ref="A105" r:id="rId104" display="http://www.corporatecouriers.com/" xr:uid="{8621FB21-D785-6244-BA82-6B07E4A071A8}"/>
+    <hyperlink ref="A106" r:id="rId105" display="http://www.smart-delivery.com/" xr:uid="{722919A5-1555-1947-B412-E4B139EA599C}"/>
+    <hyperlink ref="A107" r:id="rId106" display="http://www.cityexp.com/" xr:uid="{B161F0F5-8895-DC4C-9CC2-AAA682FABD3E}"/>
+    <hyperlink ref="A108" r:id="rId107" display="https://dedicatedlogistics.com/" xr:uid="{9A0605E8-252B-1349-8982-3CEFD005D130}"/>
+    <hyperlink ref="A109" r:id="rId108" display="http://www.firstclasscourier.com/" xr:uid="{362AF675-9AA0-2B48-A9AC-DD95A150B0A3}"/>
+    <hyperlink ref="A110" r:id="rId109" display="http://www.sprintcourier.com/" xr:uid="{493CC60E-DA46-A043-B446-2AE6141CD224}"/>
+    <hyperlink ref="A111" r:id="rId110" display="http://www.samedaydelivers.com/" xr:uid="{0434A8F6-D2E9-3D44-8D65-12B9730C2BD7}"/>
+    <hyperlink ref="A112" r:id="rId111" display="https://www.truenorthlogistics.com/" xr:uid="{46DE5B1C-8128-E242-8EB4-07D8BBEE9695}"/>
+    <hyperlink ref="A113" r:id="rId112" display="https://goshare.co/" xr:uid="{31DE32CC-3670-1941-97B3-69C074C05E05}"/>
+    <hyperlink ref="A114" r:id="rId113" display="http://www.mulesoftlogistics.com/" xr:uid="{96D3F76A-733B-DC4C-BD2F-86BDCA63F6D6}"/>
+    <hyperlink ref="A115" r:id="rId114" display="http://www.quickcourier.com/" xr:uid="{04F0F538-B5EE-2D4A-AD90-EA09C7B45C38}"/>
+    <hyperlink ref="A116" r:id="rId115" display="http://www.bonded-transportation.com/" xr:uid="{0CDDF333-6076-404C-B756-BB0B85B2FA8A}"/>
+    <hyperlink ref="A117" r:id="rId116" display="http://www.uscourier.com/" xr:uid="{29735F40-4722-A946-BAC8-923A74C6F302}"/>
+    <hyperlink ref="A118" r:id="rId117" display="http://www.expressitdelivery.com/" xr:uid="{D6AF596D-3BB5-814A-9501-A2BCAEC7B465}"/>
+    <hyperlink ref="A119" r:id="rId118" display="http://www.michiganlogistics.com/" xr:uid="{2C559D59-04BA-3648-A305-DF8DB2AC2811}"/>
+    <hyperlink ref="A120" r:id="rId119" display="http://www.easexpress.com/" xr:uid="{E6C0A4DF-4B29-6443-AB8C-0D7E8AC97BEF}"/>
+    <hyperlink ref="A121" r:id="rId120" display="http://www.sherdeltransfer.com/" xr:uid="{BB6C5ACA-C061-8240-8D44-F448DFA325BD}"/>
+    <hyperlink ref="A122" r:id="rId121" display="http://www.corporatetransit.com/" xr:uid="{D3526926-F27A-524E-9227-624BD1B37061}"/>
+    <hyperlink ref="A123" r:id="rId122" display="https://eastcoastlogistics.com/" xr:uid="{C0AE48AF-9E3D-2249-910F-D019AFB537B0}"/>
+    <hyperlink ref="A124" r:id="rId123" display="https://point2pointglobal.com/" xr:uid="{689E3A35-F35F-7C43-B50E-5CC93BBA5900}"/>
+    <hyperlink ref="A125" r:id="rId124" display="https://ecouriergroup.com/" xr:uid="{DBC1B9D8-272C-E348-9725-7ED00BCA1115}"/>
+    <hyperlink ref="A126" r:id="rId125" display="http://www.westcoastlogistics.net/" xr:uid="{DC10D6A4-C444-4E49-98DC-3489E2BCF9D4}"/>
+    <hyperlink ref="A127" r:id="rId126" display="https://www.shipmercury.com/" xr:uid="{D034C736-C615-3248-8C3B-2EBE3434CA60}"/>
+    <hyperlink ref="A128" r:id="rId127" display="https://www.ezcourier.com/" xr:uid="{16C9040A-BC17-CC45-97B5-9C5CD8DDDF8D}"/>
+    <hyperlink ref="A129" r:id="rId128" display="http://www.regionalexpressinc.com/" xr:uid="{B95E5445-9E31-3242-A954-7DDAB76BAED1}"/>
+    <hyperlink ref="A130" r:id="rId129" display="http://www.citywidecouriers.com/" xr:uid="{A30FBA8A-7528-1E4B-89F0-5FF7D173D1ED}"/>
+    <hyperlink ref="A131" r:id="rId130" display="https://www.monarchdelivery.com/" xr:uid="{6A1A2A79-1A66-C54D-9629-6926B684CC31}"/>
+    <hyperlink ref="A132" r:id="rId131" display="http://www.capitolexpressinc.com/" xr:uid="{89E9BCFC-82D6-8A43-9A30-5CB3A369A7E8}"/>
+    <hyperlink ref="A133" r:id="rId132" display="http://www.jrsexpressdelivery.com/" xr:uid="{7FDEC950-B4AA-CA4F-A1FC-8596478C50FA}"/>
+    <hyperlink ref="A134" r:id="rId133" display="https://www.acecourier.com/" xr:uid="{5A631D9C-B941-1C49-B565-F29CEA731A1D}"/>
+    <hyperlink ref="A135" r:id="rId134" display="http://www.parcelsinc.com/" xr:uid="{67312458-7442-484A-91C2-A3E626C92A1F}"/>
+    <hyperlink ref="A136" r:id="rId135" display="http://www.hollandregional.com/" xr:uid="{222F5D8B-BF76-FF48-AF9D-163F0A7269C1}"/>
+    <hyperlink ref="A137" r:id="rId136" display="http://www.prioritydispatch.com/" xr:uid="{D1AC3139-4358-6548-9998-818FE967ECFC}"/>
+    <hyperlink ref="A138" r:id="rId137" display="http://www.hackbarthdelivery.com/" xr:uid="{09764DC2-E2CF-254F-A682-0ACA6148D95E}"/>
+    <hyperlink ref="A139" r:id="rId138" display="https://www.shipgreyhound.com/" xr:uid="{458FAEF0-5C87-F042-AC78-7DB88C3EE0D4}"/>
+    <hyperlink ref="A140" r:id="rId139" display="http://www.bonneydelivery.com/" xr:uid="{1ACCF52D-5BC2-5549-BF6D-8366607790BD}"/>
+    <hyperlink ref="A141" r:id="rId140" display="http://www.shamrockexpress.com/" xr:uid="{75C59A68-676A-F649-B278-73E5ED1BF652}"/>
+    <hyperlink ref="A142" r:id="rId141" display="https://www.nationwideexpress.com/" xr:uid="{4E40ED77-558B-4148-A9E7-B1D55B27FA4B}"/>
+    <hyperlink ref="A143" r:id="rId142" display="http://www.metro-courier.com/" xr:uid="{E1C71248-40B0-9048-9175-0E86150D47F3}"/>
+    <hyperlink ref="A144" r:id="rId143" display="https://www.specializedexpress.com/" xr:uid="{2BC6C542-5FE7-1C44-A4B9-83648F9539EC}"/>
+    <hyperlink ref="A145" r:id="rId144" display="http://www.jetlinelogistics.com/" xr:uid="{3CF7FA22-5025-B24C-962A-F61DA85FAD55}"/>
+    <hyperlink ref="A146" r:id="rId145" display="http://www.swfreight.com/" xr:uid="{251B3CD1-3FCB-DD41-8F89-EC35455A7D0D}"/>
+    <hyperlink ref="A147" r:id="rId146" display="http://www.bluestreakcouriers.com/" xr:uid="{12F50950-E72F-9C4A-8515-46F56CC6F8E9}"/>
+    <hyperlink ref="A148" r:id="rId147" display="https://www.smtl.com/" xr:uid="{B62C4422-8395-2743-8C09-709ADD604246}"/>
+    <hyperlink ref="A149" r:id="rId148" display="http://www.americanlc.com/" xr:uid="{D1CAA362-9669-8042-9634-8D9329EA51A1}"/>
+    <hyperlink ref="A150" r:id="rId149" display="https://www.starfreight.com/" xr:uid="{2F0923AD-C1D4-5044-BFE6-0009D935E4A5}"/>
+    <hyperlink ref="A151" r:id="rId150" display="http://www.carey.com/" xr:uid="{97EC126C-117C-D141-B865-5445A0C376FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>